<commit_message>
added daily leet rank
</commit_message>
<xml_diff>
--- a/LeetCodeRanking.xlsx
+++ b/LeetCodeRanking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nimal\eclipse-workspace\anujSirDSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02E275C4-1749-4A29-A173-124B5C210A41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{725BF80C-8080-4806-9AB3-692B014BBA5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -60,6 +60,16 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
@@ -84,13 +94,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -371,10 +383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -408,6 +420,22 @@
         <v>1126058</v>
       </c>
     </row>
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>45084</v>
+      </c>
+      <c r="C4" s="6">
+        <v>1111777</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>45085</v>
+      </c>
+      <c r="C5" s="7">
+        <v>1083899</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added few more ranks
</commit_message>
<xml_diff>
--- a/LeetCodeRanking.xlsx
+++ b/LeetCodeRanking.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nimal\eclipse-workspace\anujSirDSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{725BF80C-8080-4806-9AB3-692B014BBA5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FFE1119-C572-4AEB-A456-70C39A6D73AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -65,6 +65,22 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
@@ -94,7 +110,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -103,6 +119,9 @@
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -383,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -436,6 +455,30 @@
         <v>1083899</v>
       </c>
     </row>
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>45086</v>
+      </c>
+      <c r="C6" s="8">
+        <v>1057863</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>45089</v>
+      </c>
+      <c r="C7" s="9">
+        <v>997429</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>45090</v>
+      </c>
+      <c r="C8" s="10">
+        <v>964202</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added non recursive tree traversals (pre-in-post)
</commit_message>
<xml_diff>
--- a/LeetCodeRanking.xlsx
+++ b/LeetCodeRanking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nimal\eclipse-workspace\anujSirDSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FFE1119-C572-4AEB-A456-70C39A6D73AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F8B9D4E-B515-4DAA-B2D9-2E3D8FE0E90E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,6 +81,41 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
@@ -110,7 +145,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -122,6 +157,13 @@
     <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -479,6 +521,62 @@
         <v>964202</v>
       </c>
     </row>
+    <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>45093</v>
+      </c>
+      <c r="C9" s="11">
+        <v>924916</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>45094</v>
+      </c>
+      <c r="C10" s="12">
+        <v>905778</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
+        <v>45095</v>
+      </c>
+      <c r="C11" s="13">
+        <v>878474</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
+        <v>45096</v>
+      </c>
+      <c r="C12" s="14">
+        <v>870259</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
+        <v>45097</v>
+      </c>
+      <c r="C13" s="15">
+        <v>836531</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
+        <v>45101</v>
+      </c>
+      <c r="C14" s="16">
+        <v>800072</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
+        <v>45103</v>
+      </c>
+      <c r="C15" s="17">
+        <v>786285</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>